<commit_message>
refactor file structure and remove all alert calls
</commit_message>
<xml_diff>
--- a/control.xlsx
+++ b/control.xlsx
@@ -1,40 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phasit/Desktop/ElectronProject/mydoc/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1CB5AA-D3FF-B240-8CC7-B631F5B1A554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15760" xr2:uid="{AF8D7D1E-3345-6647-AE73-EF79E80350AD}"/>
+    <workbookView xWindow="3540" yWindow="2250" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>ลำดับ</t>
   </si>
@@ -46,26 +26,35 @@
   </si>
   <si>
     <t>วันที่</t>
+  </si>
+  <si>
+    <t>ค่าวัสดุการศึกษา</t>
+  </si>
+  <si>
+    <t>Created on25-12-2023</t>
+  </si>
+  <si>
+    <t>2023-12-31</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
-      <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="18"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -103,13 +92,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -424,112 +419,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553FAF7E-3A6F-1A43-A77F-2D57D7427DEC}">
-  <dimension ref="A2:D12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0" zoomScale="99" zoomScaleNormal="100">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="19.5" defaultRowHeight="34" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="33.95" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25" defaultColWidth="19.42578125" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="19.5" style="1"/>
+    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="19.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+    <row r="2" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="B3" s="4"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="B4" s="4"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>5</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="B5" s="4"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="B6" s="4"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6666</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="B9" s="4"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="B11" s="4"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" ht="33.95" customHeight="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>8</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="1">
+        <v>6666</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
make input larger, add essential dependency
</commit_message>
<xml_diff>
--- a/control.xlsx
+++ b/control.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>#</t>
   </si>
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D14"/>
+  <dimension ref="A2:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
       <selection activeCell="A4" sqref="A4"/>
@@ -566,6 +566,20 @@
         <v>14</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>1234</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fix save control missing govName, thaiDate fix
</commit_message>
<xml_diff>
--- a/control.xlsx
+++ b/control.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="4020" yWindow="1950" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="4485" yWindow="1515" windowWidth="21600" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
@@ -14,11 +14,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>#</t>
   </si>
   <si>
+    <t>school</t>
+  </si>
+  <si>
     <t>detail</t>
   </si>
   <si>
@@ -59,6 +62,18 @@
   </si>
   <si>
     <t>2024-01-03</t>
+  </si>
+  <si>
+    <t>โรงเรียนเทพสถิตวิทยา</t>
+  </si>
+  <si>
+    <t>2023-12-29</t>
+  </si>
+  <si>
+    <t>โรงเรียนเขาดินพิทยารักษ์</t>
+  </si>
+  <si>
+    <t>Created on 29-12-2023</t>
   </si>
 </sst>
 </file>
@@ -376,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D15"/>
+  <dimension ref="A2:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -397,187 +412,224 @@
       <c r="D2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3">
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>324</v>
       </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
         <v>155</v>
       </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>324</v>
       </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
         <v>155</v>
       </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
         <v>2</v>
       </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7">
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
         <v>55555</v>
       </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8">
+      <c r="C8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8">
         <v>5555</v>
       </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9">
         <v>2344</v>
       </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10">
+      <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10">
         <v>12345</v>
       </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11">
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
         <v>666666</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12">
+      <c r="C12" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
         <v>123</v>
       </c>
-      <c r="D13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14">
         <v>12345</v>
       </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15">
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
         <v>1234</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
         <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>